<commit_message>
Added data to P1 node
</commit_message>
<xml_diff>
--- a/5 Lora-nodes Espressif Systems esp32/1 p1_smart_meter_TTN_Apeldoorn/esp32-p1-node-master/Settings smart meter.xlsx
+++ b/5 Lora-nodes Espressif Systems esp32/1 p1_smart_meter_TTN_Apeldoorn/esp32-p1-node-master/Settings smart meter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evers\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evers\Documents\IMAGINE-IOT\Imagine-IoT\Imagine-IoT\5 Lora-nodes Espressif Systems esp32\1 p1_smart_meter_TTN_Apeldoorn\esp32-p1-node-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F914D409-3125-44CD-8FF9-3BD800017D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF5BF47-90C7-4000-A142-415FD30A89CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C9E6696-C471-4A26-A1CC-CE63D0FB864B}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -658,7 +658,7 @@
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.2" thickBot="1">
+    <row r="1" spans="1:8" ht="21" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" thickBot="1">
+    <row r="2" spans="1:8" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -710,7 +710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="21" thickBot="1">
+    <row r="3" spans="1:8" ht="15" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -736,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" thickBot="1">
+    <row r="4" spans="1:8" ht="15" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -788,7 +788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="21" thickBot="1">
+    <row r="6" spans="1:8" ht="15" thickBot="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -800,7 +800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21" thickBot="1">
+    <row r="7" spans="1:8" ht="15" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -826,7 +826,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="31.2" thickBot="1">
+    <row r="8" spans="1:8" ht="15" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -852,7 +852,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21" thickBot="1">
+    <row r="9" spans="1:8" ht="15" thickBot="1">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -878,7 +878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="31.2" thickBot="1">
+    <row r="10" spans="1:8" ht="15" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -904,7 +904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" thickBot="1">
+    <row r="11" spans="1:8" ht="15" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -930,7 +930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="21" thickBot="1">
+    <row r="12" spans="1:8" ht="15" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -956,7 +956,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="31.2" thickBot="1">
+    <row r="13" spans="1:8" ht="21" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
@@ -982,7 +982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="21" thickBot="1">
+    <row r="14" spans="1:8" ht="15" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21" thickBot="1">
+    <row r="15" spans="1:8" ht="15" thickBot="1">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="21" thickBot="1">
+    <row r="16" spans="1:8" ht="15" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="21" thickBot="1">
+    <row r="17" spans="1:8" ht="15" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="31.2" thickBot="1">
+    <row r="18" spans="1:8" ht="21" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>42</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="41.4" thickBot="1">
+    <row r="19" spans="1:8" ht="21" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="41.4" thickBot="1">
+    <row r="20" spans="1:8" ht="21" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="20.399999999999999">
+    <row r="21" spans="1:8">
       <c r="A21" s="6" t="s">
         <v>55</v>
       </c>

</xml_diff>